<commit_message>
Add look up the marks of students according to their numbers.
</commit_message>
<xml_diff>
--- a/exceltest/模拟电子技术-performance-1523701-test.xlsx
+++ b/exceltest/模拟电子技术-performance-1523701-test.xlsx
@@ -667,7 +667,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:S46"/>
+  <dimension ref="B2:V46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -675,7 +675,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:22">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -731,7 +731,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:22">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -787,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:22">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -842,8 +842,11 @@
       <c r="S4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="V4" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="B5" t="s">
         <v>22</v>
       </c>
@@ -899,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:22">
       <c r="B6" t="s">
         <v>24</v>
       </c>
@@ -954,8 +957,11 @@
       <c r="S6" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="V6" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="B7" t="s">
         <v>26</v>
       </c>
@@ -1010,8 +1016,11 @@
       <c r="S7" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="V7" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="B8" t="s">
         <v>28</v>
       </c>
@@ -1067,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:22">
       <c r="B9" t="s">
         <v>30</v>
       </c>
@@ -1123,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:22">
       <c r="B10" t="s">
         <v>32</v>
       </c>
@@ -1178,8 +1187,11 @@
       <c r="S10" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:19">
+      <c r="V10" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -1234,8 +1246,11 @@
       <c r="S11" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="V11" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="B12" t="s">
         <v>36</v>
       </c>
@@ -1291,7 +1306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:22">
       <c r="B13" t="s">
         <v>38</v>
       </c>
@@ -1346,8 +1361,11 @@
       <c r="S13" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:19">
+      <c r="V13" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="B14" t="s">
         <v>40</v>
       </c>
@@ -1403,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:22">
       <c r="B15" t="s">
         <v>42</v>
       </c>
@@ -1459,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:22">
       <c r="B16" t="s">
         <v>44</v>
       </c>
@@ -1515,7 +1533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:22">
       <c r="B17" t="s">
         <v>46</v>
       </c>
@@ -1571,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:22">
       <c r="B18" t="s">
         <v>48</v>
       </c>
@@ -1627,7 +1645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:22">
       <c r="B19" t="s">
         <v>50</v>
       </c>
@@ -1683,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:22">
       <c r="B20" t="s">
         <v>52</v>
       </c>
@@ -1739,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:22">
       <c r="B21" t="s">
         <v>54</v>
       </c>
@@ -1795,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:22">
       <c r="B22" t="s">
         <v>56</v>
       </c>
@@ -1851,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:22">
       <c r="B23" t="s">
         <v>58</v>
       </c>
@@ -1907,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:22">
       <c r="B24" t="s">
         <v>60</v>
       </c>
@@ -1962,8 +1980,11 @@
       <c r="S24" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:19">
+      <c r="V24" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
       <c r="B25" t="s">
         <v>62</v>
       </c>
@@ -2018,8 +2039,11 @@
       <c r="S25" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:19">
+      <c r="V25" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
       <c r="B26" t="s">
         <v>64</v>
       </c>
@@ -2075,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:22">
       <c r="B27" t="s">
         <v>66</v>
       </c>
@@ -2131,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:22">
       <c r="B28" t="s">
         <v>68</v>
       </c>
@@ -2187,7 +2211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:22">
       <c r="B29" t="s">
         <v>70</v>
       </c>
@@ -2243,7 +2267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:22">
       <c r="B30" t="s">
         <v>72</v>
       </c>
@@ -2299,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:22">
       <c r="B31" t="s">
         <v>74</v>
       </c>
@@ -2355,7 +2379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:22">
       <c r="B32" t="s">
         <v>76</v>
       </c>
@@ -2411,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:22">
       <c r="B33" t="s">
         <v>78</v>
       </c>
@@ -2467,7 +2491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:22">
       <c r="B34" t="s">
         <v>80</v>
       </c>
@@ -2523,7 +2547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:22">
       <c r="B35" t="s">
         <v>82</v>
       </c>
@@ -2579,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:22">
       <c r="B36" t="s">
         <v>84</v>
       </c>
@@ -2635,7 +2659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:22">
       <c r="B37" t="s">
         <v>86</v>
       </c>
@@ -2691,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:22">
       <c r="B38" t="s">
         <v>88</v>
       </c>
@@ -2747,7 +2771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:22">
       <c r="B39" t="s">
         <v>90</v>
       </c>
@@ -2803,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:22">
       <c r="B40" t="s">
         <v>92</v>
       </c>
@@ -2859,7 +2883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:22">
       <c r="B41" t="s">
         <v>94</v>
       </c>
@@ -2915,7 +2939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:22">
       <c r="B42" t="s">
         <v>96</v>
       </c>
@@ -2971,7 +2995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:22">
       <c r="B43" t="s">
         <v>98</v>
       </c>
@@ -3027,7 +3051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:22">
       <c r="B44" t="s">
         <v>100</v>
       </c>
@@ -3083,7 +3107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:19">
+    <row r="45" spans="1:22">
       <c r="B45" t="s">
         <v>102</v>
       </c>
@@ -3139,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:19">
+    <row r="46" spans="1:22">
       <c r="B46" t="s">
         <v>104</v>
       </c>

</xml_diff>